<commit_message>
modify data for search scenario
</commit_message>
<xml_diff>
--- a/src/main/resources/archetype-resources/src/test/resources/data/in/search.xlsx
+++ b/src/main/resources/archetype-resources/src/test/resources/data/in/search.xlsx
@@ -14,27 +14,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>user</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Result</t>
   </si>
   <si>
-    <t>user1</t>
+    <t>NoraUi is open source</t>
   </si>
   <si>
-    <t>password1</t>
+    <t>search</t>
   </si>
   <si>
-    <t>user2</t>
-  </si>
-  <si>
-    <t>password2</t>
+    <t>NoraUi is free</t>
   </si>
 </sst>
 </file>
@@ -401,42 +392,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>